<commit_message>
diseño de la página principal, sección 1 y parte de la 2
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0.947516091764318</t>
+          <t>1.45098039215686</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8.125</t>
+          <t>47.0</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.552483908235682</t>
+          <t>6.45098039215686</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.06470399307259</t>
+          <t>1.04577347143334</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1.60298414312629</t>
+          <t>-1.69857747020377</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.117187901308275</t>
+          <t>0.405206920723518</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.07791209073011</t>
+          <t>0.688595493685113</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-0.180331565072615</t>
+          <t>-1.08945173217963</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0132080976575131</t>
+          <t>0.357177977748231</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.07805764787654</t>
+          <t>0.589804903444715</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.0019872259809312</t>
+          <t>-0.280218220817008</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.0001455571464379</t>
+          <t>0.0987905902403977</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,61 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.07805766521594</t>
+          <t>0.585792163076594</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-2.36726886382339e-07</t>
+          <t>-0.0113497896514318</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.73393919222775e-08</t>
+          <t>0.0040127403681217</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.585786437638495</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-1.61939844204328e-05</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>5.72543809895798e-06</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>0.585786437626905</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>-3.2781058975394394e-11</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1.1589840198666899e-11</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se agrego el metodo de vandermonde, se corrigio el metodo raices multiples para casos especificos y se organizo tabla de jacobi
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.45098039215686</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>47.0</t>
+          <t>0.25</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.45098039215686</t>
+          <t>0.5</t>
         </is>
       </c>
     </row>
@@ -485,127 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.04577347143334</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1.69857747020377</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.405206920723518</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>0.688595493685113</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>-1.08945173217963</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>0.357177977748231</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>0.589804903444715</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>-0.280218220817008</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>0.0987905902403977</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>0.585792163076594</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>-0.0113497896514318</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.0040127403681217</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0.585786437638495</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-1.61939844204328e-05</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5.72543809895798e-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0.585786437626905</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>-3.2781058975394394e-11</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1.1589840198666899e-11</t>
+          <t>0.0</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se corrige la imagen de las matrices A, x y b en jacobi
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>0.25</t>
+          <t>8.125</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.5</t>
+          <t>0.552483908235682</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,83 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2.0</t>
+          <t>0.947516091764318</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>-1.60298414312629</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.0</t>
+          <t>0.117187901308275</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.06470399307259</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>-0.180331565072615</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>0.0132080976575131</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.07791209073011</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>-0.0019872259809312</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>0.0001455571464379</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.07805764787654</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>-2.36726886382339e-07</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1.73393919222775e-08</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Método de Spline y HTML Sección 1
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>1.5</t>
+          <t>2.0</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>8.125</t>
+          <t>-9.85203026391962</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.552483908235682</t>
+          <t>1.04848751138525</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.947516091764318</t>
+          <t>0.951512488614748</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1.60298414312629</t>
+          <t>-5.70057024136476</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.117187901308275</t>
+          <t>0.428928774956478</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.06470399307259</t>
+          <t>0.52258371365827</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-0.180331565072615</t>
+          <t>-1.93462565319986</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0132080976575131</t>
+          <t>0.117995951340695</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.07791209073011</t>
+          <t>0.404587762317575</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.0019872259809312</t>
+          <t>-0.261206030131537</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.0001455571464379</t>
+          <t>0.0153770222176567</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,39 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.07805764787654</t>
+          <t>0.389210740099918</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-2.36726886382339e-07</t>
+          <t>-0.0053489238075823</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.73393919222775e-08</t>
+          <t>0.0003146487342669</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>0.388896091365651</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>-2.2901295766697e-06</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1.34716096833465e-07</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
se corrige ortografia, se hacen campos de forms obligatorios seccion 1 y 2, se agrega aprox del resultado de raices
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-5.0</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>47.0</t>
+          <t>-3.125</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>6.45098039215686</t>
+          <t>0.388707037643208</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1.45098039215686</t>
+          <t>1.88870703764321</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1.69857747020377</t>
+          <t>-0.842177693346846</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.405206920723518</t>
+          <t>0.105129720534756</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.04577347143334</t>
+          <t>1.99383675817796</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-1.08945173217963</t>
+          <t>-0.0491542264913936</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.357177977748231</t>
+          <t>0.0061442493182575</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0.688595493685113</t>
+          <t>1.99998100749622</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.280218220817008</t>
+          <t>-0.0001519385873781</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.0987905902403977</t>
+          <t>1.89923234215073e-05</t>
         </is>
       </c>
     </row>
@@ -551,61 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>0.589804903444715</t>
+          <t>1.99999999981964</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-0.0113497896514318</t>
+          <t>-1.44286005352745e-09</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.0040127403681217</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>0.585792163076594</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-1.61939844204328e-05</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>5.72543809895798e-06</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>0.585786437638495</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>-3.2781058975394394e-11</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>1.1589840198666899e-11</t>
+          <t>1.80357506707196e-10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
corrección bisección 2.0 (lectura de potencias)
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,12 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>-793.0</t>
+          <t>14.9990234375</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>5.73406534547402</t>
+          <t>2.14125859098224</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>0.734065345474023</t>
+          <t>-2.85874140901776</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-3.57803959280385</t>
+          <t>-1.8466024818928</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.26906397531866</t>
+          <t>0.289659790013761</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1.00312932079268</t>
+          <t>-3.14840119903152</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-0.962350070779876</t>
+          <t>-0.100289494253238</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0704203328586019</t>
+          <t>0.0158040433021078</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1.07354965365128</t>
+          <t>-3.16420524233363</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.0613192874469695</t>
+          <t>-0.0002491447552444</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.0044913953982159</t>
+          <t>3.92617396967054e-05</t>
         </is>
       </c>
     </row>
@@ -551,39 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>1.0780410490495</t>
+          <t>-3.16424450407332</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-0.0002268499304438</t>
+          <t>-1.52308840507432e-09</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>1.66159405259325e-05</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>1.07805766499003</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>-3.08423563379059e-09</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>2.25909069229147e-10</t>
+          <t>2.40017339336873e-10</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ultimos cambios en SOR
</commit_message>
<xml_diff>
--- a/app/tables/multiple_roots_results.xlsx
+++ b/app/tables/multiple_roots_results.xlsx
@@ -463,17 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>-5.0</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>14.9990234375</t>
+          <t>-3.125</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.14125859098224</t>
+          <t>0.388707037643208</t>
         </is>
       </c>
     </row>
@@ -485,17 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>-2.85874140901776</t>
+          <t>1.88870703764321</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>-1.8466024818928</t>
+          <t>-0.842177693346846</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.289659790013761</t>
+          <t>0.105129720534756</t>
         </is>
       </c>
     </row>
@@ -507,17 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>-3.14840119903152</t>
+          <t>1.99383675817796</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>-0.100289494253238</t>
+          <t>-0.0491542264913936</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.0158040433021078</t>
+          <t>0.0061442493182575</t>
         </is>
       </c>
     </row>
@@ -529,17 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>-3.16420524233363</t>
+          <t>1.99998100749622</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>-0.0002491447552444</t>
+          <t>-0.0001519385873781</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.92617396967054e-05</t>
+          <t>1.89923234215073e-05</t>
         </is>
       </c>
     </row>
@@ -551,17 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-3.16424450407332</t>
+          <t>1.99999999981964</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>-1.52308840507432e-09</t>
+          <t>-1.44286005352745e-09</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2.40017339336873e-10</t>
+          <t>1.80357506707196e-10</t>
         </is>
       </c>
     </row>

</xml_diff>